<commit_message>
parte do mongo feita (avaliacoes e comentarios) e outras correcoes
</commit_message>
<xml_diff>
--- a/BDII_ControloProgressoProjecto_Grupo1.xlsx
+++ b/BDII_ControloProgressoProjecto_Grupo1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Fernandes\Desktop\GitHub\BD2-Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9379ED9C-7F32-4E9D-9285-089048478837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68710067-BAF2-49E8-8F40-42EF33173532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1154,8 +1154,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>45631</v>
+        <v>45639</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -1570,11 +1570,11 @@
       <c r="E21" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="18">
-        <v>0.45</v>
+      <c r="F21" s="19">
+        <v>0.7</v>
       </c>
       <c r="G21" s="19">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1592,10 +1592,10 @@
         <v>87</v>
       </c>
       <c r="F22" s="19">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G22" s="19">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1613,10 +1613,10 @@
         <v>88</v>
       </c>
       <c r="F23" s="19">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="G23" s="19">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1634,10 +1634,10 @@
         <v>82</v>
       </c>
       <c r="F24" s="19">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="G24" s="19">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1655,10 +1655,10 @@
         <v>84</v>
       </c>
       <c r="F25" s="19">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="G25" s="19">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1675,11 +1675,11 @@
       <c r="E26" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="24">
-        <v>0</v>
+      <c r="F26" s="25">
+        <v>0.35</v>
       </c>
       <c r="G26" s="25">
-        <v>0.35</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1696,11 +1696,11 @@
       <c r="E27" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="18">
-        <v>0</v>
+      <c r="F27" s="19">
+        <v>0.7</v>
       </c>
       <c r="G27" s="19">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1717,11 +1717,11 @@
       <c r="E28" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="18">
-        <v>0</v>
+      <c r="F28" s="19">
+        <v>0.3</v>
       </c>
       <c r="G28" s="19">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1738,11 +1738,11 @@
       <c r="E29" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="18">
-        <v>0</v>
+      <c r="F29" s="19">
+        <v>0.3</v>
       </c>
       <c r="G29" s="19">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
controlo de progresso semana 8
</commit_message>
<xml_diff>
--- a/BDII_ControloProgressoProjecto_Grupo1.xlsx
+++ b/BDII_ControloProgressoProjecto_Grupo1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Fernandes\Desktop\GitHub\BD2-Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E95B107-F372-4032-AC40-0E0A825B29B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC627B35-48B1-4962-82BF-523840889E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>Data Relatório:</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>Rafael e Daniel</t>
+  </si>
+  <si>
+    <t>Francisco e Guilherme</t>
   </si>
 </sst>
 </file>
@@ -670,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -718,7 +721,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1154,8 +1156,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1181,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>45644</v>
+        <v>45645</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -1662,7 +1664,7 @@
         <v>45644</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F25" s="19">
         <v>0.8</v>
@@ -1731,7 +1733,7 @@
         <v>45644</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F28" s="19">
         <v>0.5</v>
@@ -1754,7 +1756,7 @@
         <v>45644</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F29" s="19">
         <v>0.5</v>
@@ -1773,13 +1775,17 @@
       <c r="C30" s="32">
         <v>45616</v>
       </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="30"/>
+      <c r="D30" s="32">
+        <v>45645</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>83</v>
+      </c>
       <c r="F30" s="34">
         <v>0</v>
       </c>
       <c r="G30" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1806,14 +1812,18 @@
       <c r="B32" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="16"/>
+      <c r="C32" s="27">
+        <v>45643</v>
+      </c>
       <c r="D32" s="17"/>
-      <c r="E32" s="14"/>
+      <c r="E32" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="F32" s="18">
         <v>0</v>
       </c>
       <c r="G32" s="19">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1823,72 +1833,78 @@
       <c r="B33" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="39"/>
+      <c r="C33" s="27">
+        <v>45643</v>
+      </c>
+      <c r="D33" s="37"/>
+      <c r="E33" s="38" t="s">
+        <v>82</v>
+      </c>
       <c r="F33" s="18">
         <v>0</v>
       </c>
       <c r="G33" s="19">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="42">
-        <v>0</v>
-      </c>
-      <c r="G34" s="42">
+      <c r="C34" s="32">
+        <v>45643</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="41">
+        <v>0</v>
+      </c>
+      <c r="G34" s="41">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="45">
+      <c r="C35" s="44">
         <v>45304</v>
       </c>
-      <c r="D35" s="46" t="s">
+      <c r="D35" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="43"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="42"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="52">
-        <v>0</v>
-      </c>
-      <c r="G36" s="53">
+      <c r="C36" s="48"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="51">
+        <v>0</v>
+      </c>
+      <c r="G36" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="54" t="s">
         <v>69</v>
       </c>
       <c r="C37" s="22"/>
@@ -1902,10 +1918,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="54" t="s">
         <v>71</v>
       </c>
       <c r="C38" s="22"/>
@@ -1919,10 +1935,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="55" t="s">
         <v>73</v>
       </c>
       <c r="C39" s="22"/>
@@ -1936,10 +1952,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="55" t="s">
         <v>75</v>
       </c>
       <c r="C40" s="22"/>
@@ -1953,10 +1969,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="54" t="s">
+      <c r="A41" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="55" t="s">
         <v>77</v>
       </c>
       <c r="C41" s="22"/>
@@ -1970,10 +1986,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="54" t="s">
+      <c r="A42" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="55" t="s">
         <v>79</v>
       </c>
       <c r="C42" s="22"/>
@@ -1987,19 +2003,19 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="57" t="s">
+      <c r="A43" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="59"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="62">
-        <v>0</v>
-      </c>
-      <c r="G43" s="63">
+      <c r="C43" s="58"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="61">
+        <v>0</v>
+      </c>
+      <c r="G43" s="62">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Controlo de progresso semana 9
</commit_message>
<xml_diff>
--- a/BDII_ControloProgressoProjecto_Grupo1.xlsx
+++ b/BDII_ControloProgressoProjecto_Grupo1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Fernandes\Desktop\GitHub\BD2-Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC627B35-48B1-4962-82BF-523840889E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E05555-6B96-4E97-BE8D-F02537A253EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>Data Relatório:</t>
   </si>
@@ -313,9 +313,6 @@
   </si>
   <si>
     <t>Rafael e Daniel</t>
-  </si>
-  <si>
-    <t>Francisco e Guilherme</t>
   </si>
 </sst>
 </file>
@@ -673,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -721,10 +718,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -732,7 +727,6 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -744,7 +738,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1156,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1181,7 +1174,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>45645</v>
+        <v>45657</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -1575,7 +1568,7 @@
         <v>84</v>
       </c>
       <c r="F21" s="19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G21" s="19">
         <v>1</v>
@@ -1598,7 +1591,7 @@
         <v>87</v>
       </c>
       <c r="F22" s="19">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G22" s="19">
         <v>1</v>
@@ -1621,7 +1614,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G23" s="19">
         <v>1</v>
@@ -1644,7 +1637,7 @@
         <v>82</v>
       </c>
       <c r="F24" s="19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G24" s="19">
         <v>1</v>
@@ -1667,7 +1660,7 @@
         <v>85</v>
       </c>
       <c r="F25" s="19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G25" s="19">
         <v>1</v>
@@ -1689,8 +1682,8 @@
       <c r="E26" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="25">
-        <v>0.65</v>
+      <c r="F26" s="19">
+        <v>1</v>
       </c>
       <c r="G26" s="19">
         <v>1</v>
@@ -1713,7 +1706,7 @@
         <v>94</v>
       </c>
       <c r="F27" s="19">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G27" s="19">
         <v>1</v>
@@ -1736,7 +1729,7 @@
         <v>83</v>
       </c>
       <c r="F28" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G28" s="19">
         <v>1</v>
@@ -1759,7 +1752,7 @@
         <v>88</v>
       </c>
       <c r="F29" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G29" s="19">
         <v>1</v>
@@ -1782,7 +1775,7 @@
         <v>83</v>
       </c>
       <c r="F30" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="35">
         <v>1</v>
@@ -1815,15 +1808,17 @@
       <c r="C32" s="27">
         <v>45643</v>
       </c>
-      <c r="D32" s="17"/>
+      <c r="D32" s="27">
+        <v>45649</v>
+      </c>
       <c r="E32" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F32" s="18">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="F32" s="19">
+        <v>0.3</v>
       </c>
       <c r="G32" s="19">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1836,78 +1831,90 @@
       <c r="C33" s="27">
         <v>45643</v>
       </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="18">
-        <v>0</v>
+      <c r="D33" s="27">
+        <v>45649</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="19">
+        <v>0.2</v>
       </c>
       <c r="G33" s="19">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="38" t="s">
         <v>62</v>
       </c>
       <c r="C34" s="32">
         <v>45643</v>
       </c>
-      <c r="D34" s="40"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="41">
+      <c r="D34" s="32">
+        <v>45657</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="39">
         <v>0</v>
       </c>
-      <c r="G34" s="41">
+      <c r="G34" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="42">
+        <v>45304</v>
+      </c>
+      <c r="D35" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="40"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="40"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="27">
+        <v>45657</v>
+      </c>
+      <c r="D36" s="46"/>
+      <c r="E36" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="44">
-        <v>45304</v>
-      </c>
-      <c r="D35" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="42"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="42"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="51">
-        <v>0</v>
-      </c>
-      <c r="G36" s="52">
-        <v>0</v>
+      <c r="G36" s="49">
+        <v>0.3</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="22"/>
+      <c r="C37" s="27">
+        <v>45657</v>
+      </c>
       <c r="D37" s="23"/>
       <c r="E37" s="20"/>
       <c r="F37" s="24">
@@ -1918,13 +1925,15 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="22"/>
+      <c r="C38" s="27">
+        <v>45657</v>
+      </c>
       <c r="D38" s="23"/>
       <c r="E38" s="20"/>
       <c r="F38" s="24">
@@ -1935,64 +1944,84 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="55" t="s">
+      <c r="B39" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="20"/>
+      <c r="C39" s="27">
+        <v>45657</v>
+      </c>
+      <c r="D39" s="27">
+        <v>45657</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>83</v>
+      </c>
       <c r="F39" s="24">
         <v>0</v>
       </c>
       <c r="G39" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="53" t="s">
+      <c r="A40" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="20"/>
+      <c r="C40" s="27">
+        <v>45657</v>
+      </c>
+      <c r="D40" s="27">
+        <v>45657</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="F40" s="24">
         <v>0</v>
       </c>
       <c r="G40" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="20"/>
+      <c r="C41" s="27">
+        <v>45657</v>
+      </c>
+      <c r="D41" s="27">
+        <v>45657</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="F41" s="24">
         <v>0</v>
       </c>
       <c r="G41" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="53" t="s">
+      <c r="A42" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="55" t="s">
+      <c r="B42" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="22"/>
+      <c r="C42" s="27">
+        <v>45657</v>
+      </c>
       <c r="D42" s="23"/>
       <c r="E42" s="20"/>
       <c r="F42" s="24">
@@ -2002,20 +2031,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="56" t="s">
+    <row r="43" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="57" t="s">
+      <c r="B43" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="58"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="61">
+      <c r="C43" s="32">
+        <v>45657</v>
+      </c>
+      <c r="D43" s="55"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="57">
         <v>0</v>
       </c>
-      <c r="G43" s="62">
+      <c r="G43" s="58">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Controlo de progresso semana 10
</commit_message>
<xml_diff>
--- a/BDII_ControloProgressoProjecto_Grupo1.xlsx
+++ b/BDII_ControloProgressoProjecto_Grupo1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Fernandes\Desktop\GitHub\BD2-Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E05555-6B96-4E97-BE8D-F02537A253EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33124607-380F-4F1D-9D50-32BBBD995DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -670,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -729,7 +729,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -1149,8 +1148,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1174,7 +1173,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>45657</v>
+        <v>45665</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -1899,17 +1898,17 @@
         <v>84</v>
       </c>
       <c r="F36" s="48">
-        <v>0</v>
-      </c>
-      <c r="G36" s="49">
         <v>0.3</v>
       </c>
+      <c r="G36" s="48">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="50" t="s">
         <v>69</v>
       </c>
       <c r="C37" s="27">
@@ -1925,10 +1924,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="50" t="s">
         <v>71</v>
       </c>
       <c r="C38" s="27">
@@ -1944,10 +1943,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="50" t="s">
+      <c r="A39" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="52" t="s">
+      <c r="B39" s="51" t="s">
         <v>73</v>
       </c>
       <c r="C39" s="27">
@@ -1959,18 +1958,18 @@
       <c r="E39" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="24">
-        <v>0</v>
+      <c r="F39" s="25">
+        <v>1</v>
       </c>
       <c r="G39" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="51" t="s">
         <v>75</v>
       </c>
       <c r="C40" s="27">
@@ -1982,18 +1981,18 @@
       <c r="E40" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F40" s="24">
-        <v>0</v>
+      <c r="F40" s="25">
+        <v>1</v>
       </c>
       <c r="G40" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="51" t="s">
         <v>77</v>
       </c>
       <c r="C41" s="27">
@@ -2005,18 +2004,18 @@
       <c r="E41" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F41" s="24">
-        <v>0</v>
+      <c r="F41" s="25">
+        <v>1</v>
       </c>
       <c r="G41" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="52" t="s">
+      <c r="B42" s="51" t="s">
         <v>79</v>
       </c>
       <c r="C42" s="27">
@@ -2032,21 +2031,21 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="53" t="s">
         <v>81</v>
       </c>
       <c r="C43" s="32">
         <v>45657</v>
       </c>
-      <c r="D43" s="55"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="57">
+      <c r="D43" s="54"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="56">
         <v>0</v>
       </c>
-      <c r="G43" s="58">
+      <c r="G43" s="57">
         <v>0</v>
       </c>
     </row>

</xml_diff>